<commit_message>
prepare the seeds and parse data form csv file function
</commit_message>
<xml_diff>
--- a/src/seeds/files/001_MalaUva_SeedFile.xlsx
+++ b/src/seeds/files/001_MalaUva_SeedFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nama/Library/CloudStorage/Dropbox/00-WF-C/2-NAMA/ROCKTHECODE/CODE/02-deliverables/22_RTC_P13_backend-react/malauva-backend/src/seeds/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C452347-7D9F-5844-B0FA-D62230542DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6A7F18-0033-FB4F-9B7F-1F02736710E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120260" yWindow="-8340" windowWidth="24720" windowHeight="21420" activeTab="2" xr2:uid="{52677FAD-7042-B148-9A25-30607DD347FB}"/>
+    <workbookView xWindow="120260" yWindow="-8340" windowWidth="24720" windowHeight="21420" activeTab="1" xr2:uid="{52677FAD-7042-B148-9A25-30607DD347FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Wines" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="229">
   <si>
     <t>name</t>
   </si>
@@ -722,6 +722,9 @@
   </si>
   <si>
     <t>date 24</t>
+  </si>
+  <si>
+    <t>username</t>
   </si>
 </sst>
 </file>
@@ -1423,15 +1426,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F341AF76-375D-CC4F-BE34-40B60AD74311}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:D23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>228</v>
       </c>
       <c r="B1" t="s">
         <v>47</v>
@@ -1465,6 +1466,9 @@
       <c r="C2" t="s">
         <v>56</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
       <c r="E2" t="s">
         <v>57</v>
       </c>
@@ -1485,6 +1489,9 @@
       <c r="C3" t="s">
         <v>56</v>
       </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
       <c r="E3" t="s">
         <v>60</v>
       </c>
@@ -1505,6 +1512,9 @@
       <c r="C4" t="s">
         <v>56</v>
       </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
       <c r="E4" t="s">
         <v>63</v>
       </c>
@@ -1525,6 +1535,9 @@
       <c r="C5" t="s">
         <v>56</v>
       </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
       <c r="E5" t="s">
         <v>66</v>
       </c>
@@ -1545,6 +1558,9 @@
       <c r="C6" t="s">
         <v>56</v>
       </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
       <c r="E6" t="s">
         <v>69</v>
       </c>
@@ -1565,6 +1581,9 @@
       <c r="C7" t="s">
         <v>56</v>
       </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
       <c r="E7" t="s">
         <v>72</v>
       </c>
@@ -1585,6 +1604,9 @@
       <c r="C8" t="s">
         <v>56</v>
       </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
       <c r="E8" t="s">
         <v>75</v>
       </c>
@@ -1605,6 +1627,9 @@
       <c r="C9" t="s">
         <v>56</v>
       </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
       <c r="E9" t="s">
         <v>78</v>
       </c>
@@ -1625,6 +1650,9 @@
       <c r="C10" t="s">
         <v>56</v>
       </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
       <c r="E10" t="s">
         <v>81</v>
       </c>
@@ -1645,6 +1673,9 @@
       <c r="C11" t="s">
         <v>56</v>
       </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
       <c r="E11" t="s">
         <v>84</v>
       </c>
@@ -1664,6 +1695,9 @@
       </c>
       <c r="C12" t="s">
         <v>56</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
       </c>
       <c r="E12" t="s">
         <v>87</v>
@@ -1752,7 +1786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{457D69DA-3C5E-F74C-8219-2AB83CD0093A}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
prepare seeds and feed scripts
</commit_message>
<xml_diff>
--- a/src/seeds/files/001_MalaUva_SeedFile.xlsx
+++ b/src/seeds/files/001_MalaUva_SeedFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nama/Library/CloudStorage/Dropbox/00-WF-C/2-NAMA/ROCKTHECODE/CODE/02-deliverables/22_RTC_P13_backend-react/malauva-backend/src/seeds/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6A7F18-0033-FB4F-9B7F-1F02736710E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13070D8E-453C-8542-B340-D879A1A9E909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120260" yWindow="-8340" windowWidth="24720" windowHeight="21420" activeTab="1" xr2:uid="{52677FAD-7042-B148-9A25-30607DD347FB}"/>
+    <workbookView xWindow="120260" yWindow="-8340" windowWidth="24720" windowHeight="21420" xr2:uid="{52677FAD-7042-B148-9A25-30607DD347FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Wines" sheetId="1" r:id="rId1"/>
@@ -1095,7 +1095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A720E99C-703D-DB41-BD15-61F7B367C044}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1426,7 +1426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F341AF76-375D-CC4F-BE34-40B60AD74311}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1787,7 +1787,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>